<commit_message>
Cleaning of columns reco by Raja
</commit_message>
<xml_diff>
--- a/Data_Dictionary_Raja_Analysed.xlsx
+++ b/Data_Dictionary_Raja_Analysed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Selva\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SKA9COB\Desktop\CaseStudy\LendingClubPvt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFE8FF5-ACBB-45B8-8705-B02E8688CB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C920C103-7274-4448-AE8B-92A42D0E3B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="249">
   <si>
     <t>id</t>
   </si>
@@ -772,6 +772,12 @@
   </si>
   <si>
     <t>total_bc_limit</t>
+  </si>
+  <si>
+    <t>Analysis Remarks</t>
+  </si>
+  <si>
+    <t>Same value in all fields</t>
   </si>
 </sst>
 </file>
@@ -1510,7 +1516,15 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1536,8 +1550,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="2"/>
+      <tableStyleElement type="headerRow" dxfId="1"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1838,34 +1852,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:V118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="196.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="118.77734375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="30.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="196.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="118.81640625" style="6" customWidth="1"/>
     <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>94</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>48</v>
       </c>
+      <c r="C1" s="6" t="s">
+        <v>247</v>
+      </c>
       <c r="V1" s="23"/>
     </row>
-    <row r="2" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>229</v>
       </c>
@@ -1874,7 +1891,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>233</v>
       </c>
@@ -1883,7 +1900,7 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -1892,7 +1909,7 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>223</v>
       </c>
@@ -1901,7 +1918,7 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -1910,7 +1927,7 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>191</v>
       </c>
@@ -1919,16 +1936,18 @@
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="26" t="s">
         <v>189</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:22" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" s="4" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>108</v>
       </c>
@@ -1937,7 +1956,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>234</v>
       </c>
@@ -1946,7 +1965,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:22" s="5" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" s="5" customFormat="1" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>235</v>
       </c>
@@ -1955,7 +1974,7 @@
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>99</v>
       </c>
@@ -1964,7 +1983,7 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>165</v>
       </c>
@@ -1973,16 +1992,18 @@
       </c>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="24" t="s">
         <v>100</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="21" t="s">
         <v>22</v>
       </c>
@@ -1991,7 +2012,7 @@
       </c>
       <c r="C15" s="20"/>
     </row>
-    <row r="16" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>236</v>
       </c>
@@ -2000,7 +2021,7 @@
       </c>
       <c r="C16" s="20"/>
     </row>
-    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="24" t="s">
         <v>17</v>
       </c>
@@ -2009,7 +2030,7 @@
       </c>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:3" s="4" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" s="4" customFormat="1" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -2018,7 +2039,7 @@
       </c>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>192</v>
       </c>
@@ -2027,7 +2048,7 @@
       </c>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
@@ -2036,7 +2057,7 @@
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>10</v>
       </c>
@@ -2045,7 +2066,7 @@
       </c>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>154</v>
       </c>
@@ -2054,7 +2075,7 @@
       </c>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>25</v>
       </c>
@@ -2063,7 +2084,7 @@
       </c>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
@@ -2072,7 +2093,7 @@
       </c>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
@@ -2081,7 +2102,7 @@
       </c>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
@@ -2090,7 +2111,7 @@
       </c>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="27" t="s">
         <v>8</v>
       </c>
@@ -2099,7 +2120,7 @@
       </c>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>11</v>
       </c>
@@ -2108,7 +2129,7 @@
       </c>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>0</v>
       </c>
@@ -2117,7 +2138,7 @@
       </c>
       <c r="C29" s="20"/>
     </row>
-    <row r="30" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
         <v>215</v>
       </c>
@@ -2126,7 +2147,7 @@
       </c>
       <c r="C30" s="20"/>
     </row>
-    <row r="31" spans="1:3" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" s="4" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>34</v>
       </c>
@@ -2135,7 +2156,7 @@
       </c>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
         <v>225</v>
       </c>
@@ -2144,7 +2165,7 @@
       </c>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
         <v>227</v>
       </c>
@@ -2153,7 +2174,7 @@
       </c>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>26</v>
       </c>
@@ -2162,7 +2183,7 @@
       </c>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -2171,7 +2192,7 @@
       </c>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>6</v>
       </c>
@@ -2180,7 +2201,7 @@
       </c>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>13</v>
       </c>
@@ -2191,7 +2212,7 @@
       <c r="I37" s="10"/>
       <c r="J37" s="11"/>
     </row>
-    <row r="38" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -2200,7 +2221,7 @@
       </c>
       <c r="C38" s="5"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>46</v>
       </c>
@@ -2209,7 +2230,7 @@
       </c>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>47</v>
       </c>
@@ -2218,7 +2239,7 @@
       </c>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>43</v>
       </c>
@@ -2227,7 +2248,7 @@
       </c>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>42</v>
       </c>
@@ -2236,7 +2257,7 @@
       </c>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
@@ -2245,7 +2266,7 @@
       </c>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>14</v>
       </c>
@@ -2254,7 +2275,7 @@
       </c>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>221</v>
       </c>
@@ -2263,7 +2284,7 @@
       </c>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>1</v>
       </c>
@@ -2275,7 +2296,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
         <v>237</v>
       </c>
@@ -2287,7 +2308,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="11"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
         <v>118</v>
       </c>
@@ -2299,7 +2320,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="11"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
         <v>119</v>
       </c>
@@ -2308,7 +2329,7 @@
       </c>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
         <v>105</v>
       </c>
@@ -2317,7 +2338,7 @@
       </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
         <v>238</v>
       </c>
@@ -2326,7 +2347,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="21" t="s">
         <v>27</v>
       </c>
@@ -2335,7 +2356,7 @@
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="8" t="s">
         <v>102</v>
       </c>
@@ -2344,7 +2365,7 @@
       </c>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>28</v>
       </c>
@@ -2353,7 +2374,7 @@
       </c>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
         <v>211</v>
       </c>
@@ -2362,7 +2383,7 @@
       </c>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
         <v>239</v>
       </c>
@@ -2371,7 +2392,7 @@
       </c>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="8" t="s">
         <v>240</v>
       </c>
@@ -2380,7 +2401,7 @@
       </c>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="s">
         <v>242</v>
       </c>
@@ -2389,7 +2410,7 @@
       </c>
       <c r="D58" s="4"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
         <v>243</v>
       </c>
@@ -2398,7 +2419,7 @@
       </c>
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="24" t="s">
         <v>44</v>
       </c>
@@ -2407,7 +2428,7 @@
       </c>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
         <v>98</v>
       </c>
@@ -2416,7 +2437,7 @@
       </c>
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
         <v>110</v>
       </c>
@@ -2424,7 +2445,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
         <v>117</v>
       </c>
@@ -2432,7 +2453,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="9" t="s">
         <v>111</v>
       </c>
@@ -2440,7 +2461,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="9" t="s">
         <v>109</v>
       </c>
@@ -2448,7 +2469,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
         <v>116</v>
       </c>
@@ -2456,7 +2477,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="9" t="s">
         <v>121</v>
       </c>
@@ -2464,7 +2485,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="9" t="s">
         <v>96</v>
       </c>
@@ -2472,7 +2493,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="9" t="s">
         <v>120</v>
       </c>
@@ -2480,7 +2501,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="9" t="s">
         <v>103</v>
       </c>
@@ -2488,7 +2509,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="9" t="s">
         <v>115</v>
       </c>
@@ -2496,7 +2517,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
         <v>114</v>
       </c>
@@ -2504,7 +2525,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="9" t="s">
         <v>113</v>
       </c>
@@ -2514,7 +2535,7 @@
       <c r="C73"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="9" t="s">
         <v>104</v>
       </c>
@@ -2522,7 +2543,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>29</v>
       </c>
@@ -2530,7 +2551,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="9" t="s">
         <v>203</v>
       </c>
@@ -2538,7 +2559,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="9" t="s">
         <v>207</v>
       </c>
@@ -2546,7 +2567,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="9" t="s">
         <v>209</v>
       </c>
@@ -2554,7 +2575,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="9" t="s">
         <v>205</v>
       </c>
@@ -2562,7 +2583,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="9" t="s">
         <v>217</v>
       </c>
@@ -2570,7 +2591,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="9" t="s">
         <v>219</v>
       </c>
@@ -2578,7 +2599,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="21" t="s">
         <v>35</v>
       </c>
@@ -2586,7 +2607,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>36</v>
       </c>
@@ -2594,7 +2615,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="9" t="s">
         <v>112</v>
       </c>
@@ -2602,7 +2623,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="9" t="s">
         <v>244</v>
       </c>
@@ -2610,7 +2631,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A86" s="24" t="s">
         <v>123</v>
       </c>
@@ -2618,7 +2639,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="21" t="s">
         <v>30</v>
       </c>
@@ -2626,7 +2647,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="25" t="s">
         <v>97</v>
       </c>
@@ -2634,7 +2655,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="27" t="s">
         <v>18</v>
       </c>
@@ -2642,7 +2663,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="24" t="s">
         <v>15</v>
       </c>
@@ -2650,7 +2671,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="7" t="s">
         <v>164</v>
       </c>
@@ -2658,7 +2679,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="21" t="s">
         <v>31</v>
       </c>
@@ -2666,7 +2687,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="21" t="s">
         <v>32</v>
       </c>
@@ -2674,7 +2695,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
         <v>9</v>
       </c>
@@ -2682,7 +2703,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" s="9" t="s">
         <v>101</v>
       </c>
@@ -2690,7 +2711,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
         <v>5</v>
       </c>
@@ -2698,7 +2719,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="24" t="s">
         <v>19</v>
       </c>
@@ -2706,7 +2727,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="9" t="s">
         <v>122</v>
       </c>
@@ -2714,7 +2735,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="9" t="s">
         <v>107</v>
       </c>
@@ -2722,7 +2743,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" s="9" t="s">
         <v>106</v>
       </c>
@@ -2730,7 +2751,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" s="21" t="s">
         <v>33</v>
       </c>
@@ -2738,7 +2759,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="9" t="s">
         <v>245</v>
       </c>
@@ -2746,7 +2767,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" s="9" t="s">
         <v>213</v>
       </c>
@@ -2754,7 +2775,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" s="9" t="s">
         <v>246</v>
       </c>
@@ -2762,7 +2783,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" s="9" t="s">
         <v>231</v>
       </c>
@@ -2770,7 +2791,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" s="9" t="s">
         <v>95</v>
       </c>
@@ -2778,7 +2799,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
         <v>37</v>
       </c>
@@ -2786,7 +2807,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
         <v>38</v>
       </c>
@@ -2794,7 +2815,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
         <v>40</v>
       </c>
@@ -2802,7 +2823,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
         <v>41</v>
       </c>
@@ -2810,7 +2831,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
         <v>39</v>
       </c>
@@ -2818,7 +2839,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" s="9" t="s">
         <v>158</v>
       </c>
@@ -2826,7 +2847,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" s="24" t="s">
         <v>16</v>
       </c>
@@ -2834,7 +2855,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" s="7" t="s">
         <v>232</v>
       </c>
@@ -2842,7 +2863,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" s="7" t="s">
         <v>194</v>
       </c>
@@ -2850,7 +2871,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" s="16" t="s">
         <v>184</v>
       </c>
@@ -2858,13 +2879,17 @@
         <v>183</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B118" s="13" t="s">
         <v>156</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B116" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:B116" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <colorFilter dxfId="0" cellColor="0"/>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B101">
     <sortCondition ref="A2:A101"/>
   </sortState>
@@ -2881,13 +2906,13 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="225.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="225.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>166</v>
       </c>
@@ -2895,7 +2920,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
         <v>167</v>
       </c>
@@ -2903,7 +2928,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>168</v>
       </c>
@@ -2911,7 +2936,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
         <v>169</v>
       </c>
@@ -2919,7 +2944,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>180</v>
       </c>
@@ -2927,7 +2952,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>170</v>
       </c>
@@ -2935,7 +2960,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>182</v>
       </c>
@@ -2943,7 +2968,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>171</v>
       </c>
@@ -2951,7 +2976,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
         <v>172</v>
       </c>
@@ -2959,7 +2984,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
         <v>173</v>
       </c>
@@ -2967,11 +2992,11 @@
         <v>177</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="18"/>
       <c r="B12" s="19"/>
     </row>

</xml_diff>